<commit_message>
write to excel done
</commit_message>
<xml_diff>
--- a/src/test/resources/Run_Manager_SAKANI_4.xlsx
+++ b/src/test/resources/Run_Manager_SAKANI_4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\CrewCentricPOM2023-nhcAutomationSuiteToma\CrewCentricPOM2023-nhcAutomationSuiteToma\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\NHC_SAKANI_R4\SAKANI_3-4\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC38013-6499-41D0-A9B4-5409AF0ECC69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D298B453-D1BB-4A6D-A8EF-1C04F262CA61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="259">
   <si>
     <t>P_Key</t>
   </si>
@@ -801,6 +801,9 @@
   </si>
   <si>
     <t>Registration/Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No </t>
   </si>
 </sst>
 </file>
@@ -1575,7 +1578,7 @@
       <selection activeCell="G5" sqref="G5"/>
       <selection pane="topRight" activeCell="G5" sqref="G5"/>
       <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1718,7 +1721,7 @@
         <v>14</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>43</v>
+        <v>258</v>
       </c>
       <c r="K4" s="2">
         <v>1</v>

</xml_diff>